<commit_message>
Analysis - Calculated the survival rate of the passangers
</commit_message>
<xml_diff>
--- a/Titanic.xlsx
+++ b/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshr\Desktop\Data analytics\Excel\Excel-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2B7974-B420-4A2E-A849-1BF21707AD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF8180-16C0-496E-A918-3814949E0A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35295,10 +35295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA9C3FA-328B-4B7E-8BC0-43999772E7D0}">
-  <dimension ref="A1:K892"/>
+  <dimension ref="A1:K895"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A877" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E902" sqref="E902"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35380,9 +35380,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -67411,6 +67409,24 @@
       </c>
       <c r="K892" s="1" t="s">
         <v>1226</v>
+      </c>
+    </row>
+    <row r="893" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B893">
+        <f>COUNT(B2:B892)</f>
+        <v>891</v>
+      </c>
+    </row>
+    <row r="894" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B894">
+        <f xml:space="preserve"> COUNTIF(B2:B892, "=1")</f>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="895" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B895">
+        <f xml:space="preserve"> (B894/B893) * 100</f>
+        <v>38.383838383838381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analysis - The average age of the people onboard
</commit_message>
<xml_diff>
--- a/Titanic.xlsx
+++ b/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshr\Desktop\Data analytics\Excel\Excel-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF8180-16C0-496E-A918-3814949E0A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F850C8-6B1D-413C-BA23-04AA9D926B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35297,8 +35297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA9C3FA-328B-4B7E-8BC0-43999772E7D0}">
   <dimension ref="A1:K895"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A877" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E902" sqref="E902"/>
+    <sheetView tabSelected="1" topLeftCell="A861" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F894" sqref="F894"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -67416,6 +67416,10 @@
         <f>COUNT(B2:B892)</f>
         <v>891</v>
       </c>
+      <c r="F893">
+        <f>AVERAGE(F2:F892)</f>
+        <v>29.579315375982041</v>
+      </c>
     </row>
     <row r="894" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B894">

</xml_diff>

<commit_message>
Analysis - Calculated the proportion of males and females onboard
</commit_message>
<xml_diff>
--- a/Titanic.xlsx
+++ b/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshr\Desktop\Data analytics\Excel\Excel-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F850C8-6B1D-413C-BA23-04AA9D926B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0486944-6709-48D4-8702-D16DCB185439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3761,9 +3761,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3984,8 +3985,8 @@
   </sheetPr>
   <dimension ref="A1:L892"/>
   <sheetViews>
-    <sheetView topLeftCell="C860" workbookViewId="0">
-      <selection activeCell="M869" sqref="M869"/>
+    <sheetView topLeftCell="A872" workbookViewId="0">
+      <selection activeCell="H894" sqref="H894"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -35297,8 +35298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA9C3FA-328B-4B7E-8BC0-43999772E7D0}">
   <dimension ref="A1:K895"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A861" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F894" sqref="F894"/>
+    <sheetView tabSelected="1" topLeftCell="A879" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G898" sqref="G898"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -67416,6 +67417,10 @@
         <f>COUNT(B2:B892)</f>
         <v>891</v>
       </c>
+      <c r="E893" s="2">
+        <f>COUNTIF(E2:E892, "=male") / COUNTIF(E2:E892, "=female")</f>
+        <v>1.8375796178343948</v>
+      </c>
       <c r="F893">
         <f>AVERAGE(F2:F892)</f>
         <v>29.579315375982041</v>

</xml_diff>

<commit_message>
Analysis - Checked the class of passangers who had the highest survival rate
</commit_message>
<xml_diff>
--- a/Titanic.xlsx
+++ b/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshr\Desktop\Data analytics\Excel\Excel-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0486944-6709-48D4-8702-D16DCB185439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10438A93-C168-43BB-8FBD-6D26452E8512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35298,8 +35298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA9C3FA-328B-4B7E-8BC0-43999772E7D0}">
   <dimension ref="A1:K895"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A879" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G898" sqref="G898"/>
+    <sheetView tabSelected="1" topLeftCell="A887" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C896" sqref="C896"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -67417,6 +67417,10 @@
         <f>COUNT(B2:B892)</f>
         <v>891</v>
       </c>
+      <c r="C893">
+        <f>COUNTIFS(C2:C892, "=3", B2:B892, "=1")</f>
+        <v>119</v>
+      </c>
       <c r="E893" s="2">
         <f>COUNTIF(E2:E892, "=male") / COUNTIF(E2:E892, "=female")</f>
         <v>1.8375796178343948</v>
@@ -67431,12 +67435,20 @@
         <f xml:space="preserve"> COUNTIF(B2:B892, "=1")</f>
         <v>342</v>
       </c>
+      <c r="C894">
+        <f>COUNTIFS(C2:C892, "=2", B2:B892, "=1")</f>
+        <v>87</v>
+      </c>
     </row>
     <row r="895" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B895">
         <f xml:space="preserve"> (B894/B893) * 100</f>
         <v>38.383838383838381</v>
       </c>
+      <c r="C895">
+        <f>COUNTIFS(C2:C892, "=1", B2:B892, "=1")</f>
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>